<commit_message>
Everything currently works sanity push
</commit_message>
<xml_diff>
--- a/RESULTS/Latest results/Results_Spreadsheet.xlsx
+++ b/RESULTS/Latest results/Results_Spreadsheet.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d20867f98547c38/Documents/University/2022/SEMESTER 2/ELEN4002_EIEInvestigation/REPO/EIE-Investigation-22G05/RESULTS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d20867f98547c38/Documents/University/2022/SEMESTER 2/ELEN4002_EIEInvestigation/REPO/EIE-Investigation-22G05/RESULTS/Latest results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{89425EF1-4973-4996-A676-94CC1596E7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:40009_{89425EF1-4973-4996-A676-94CC1596E7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{055E65F7-1F24-44A1-93CB-706005097551}"/>
   <bookViews>
-    <workbookView xWindow="-1830" yWindow="2160" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="38280" yWindow="2415" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="D_Determinant2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -55,8 +68,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,8 +204,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,6 +398,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -539,9 +565,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -609,6 +637,1709 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>D_Determinant2!$B$127:$D$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>51.270530283648597</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.3543865967508</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88.507875442856701</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0A98-4DB6-9C45-2FFB0F40C257}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="316847151"/>
+        <c:axId val="316845903"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="316847151"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="316845903"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="316845903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="316847151"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>D_Determinant2!$M$127:$Q$127</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>60.712261384362002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.382400265335299</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.524006465592699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.226307771847001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.3413037897995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0E80-413C-BCD9-9F003FA91297}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="487373231"/>
+        <c:axId val="324421567"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="487373231"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="324421567"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="324421567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="487373231"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0634BA20-BBE2-7665-4457-8596F362470C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{172B2473-2B7B-DD01-F3F3-71FE1DCC0831}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -907,12 +2638,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U127"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M38" sqref="M38"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M128" sqref="M128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,6 +3292,7 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
       <c r="L20" s="1">
         <v>20</v>
       </c>
@@ -1713,6 +3445,9 @@
         <v>153.410871257916</v>
       </c>
     </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+    </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>27</v>
@@ -1769,6 +3504,7 @@
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
       <c r="L29" s="1">
         <v>29</v>
       </c>
@@ -1777,6 +3513,7 @@
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
       <c r="L30" s="1">
         <v>30</v>
       </c>
@@ -2104,6 +3841,7 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
       <c r="L42" s="1">
         <v>42</v>
       </c>
@@ -2370,6 +4108,9 @@
         <v>82.639977016166398</v>
       </c>
     </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+    </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>52</v>
@@ -2420,6 +4161,9 @@
         <v>51.553641594970799</v>
       </c>
     </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+    </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>54</v>
@@ -2467,6 +4211,7 @@
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
       <c r="L56" s="1">
         <v>56</v>
       </c>
@@ -2492,6 +4237,7 @@
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
       <c r="L58" s="1">
         <v>58</v>
       </c>
@@ -2543,11 +4289,13 @@
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
       <c r="L61" s="1">
         <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
       <c r="L62" s="1">
         <v>62</v>
       </c>
@@ -4713,6 +6461,16 @@
       </c>
       <c r="Q127">
         <v>12.3413037897995</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <f>COUNT(B2:B127)</f>
+        <v>100</v>
+      </c>
+      <c r="M128">
+        <f>COUNT(M2:M127)</f>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -4725,5 +6483,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>